<commit_message>
Module Information screen now scrollable to allow visibility on small screens. Login screen now fits on smaller screens. Register screen now fits on smaller screens. UI touch-up for grade calculator screen for small screens Grade calculator now uses database to access module credits.
Updated Task sheet to include GitHub graphs.
</commit_message>
<xml_diff>
--- a/Designs/Task Sheet.xlsx
+++ b/Designs/Task Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khiza\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khiza\Desktop\group-project-2019-20-group-26\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9988E61D-C89D-4C2D-9F2D-3EFDFEAD7D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606CB7F0-32CF-45D6-A114-380339C76F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30060" yWindow="3435" windowWidth="16635" windowHeight="17445" xr2:uid="{FFAD4A21-2BAE-4DA4-994C-E322BB9135D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FFAD4A21-2BAE-4DA4-994C-E322BB9135D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Database: users</t>
+  </si>
+  <si>
+    <t>vshaji: Vignesh</t>
+  </si>
+  <si>
+    <t>Khizar413: Khizar</t>
+  </si>
+  <si>
+    <t>R4dz: Augustas</t>
   </si>
 </sst>
 </file>
@@ -268,6 +277,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>608725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>160971</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7338027F-9818-4B41-A193-A54BB560D3CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect t="11612"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7477125" y="276225"/>
+          <a:ext cx="7000000" cy="6742746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3166D5C7-8388-4BCC-9038-8D2843B5290D}">
-  <dimension ref="C3:E31"/>
+  <dimension ref="C3:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +636,10 @@
     <col min="3" max="3" width="50.85546875" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,7 +648,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
@@ -598,31 +656,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
@@ -630,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -638,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
@@ -646,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
@@ -654,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
@@ -662,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
@@ -670,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
@@ -678,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
@@ -686,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
@@ -817,5 +884,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>